<commit_message>
updated add vacancy test and run with data driven test
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swaranjeetdhaliwal/IdeaProjects/SeleniumFramework/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933FF0EA-4A28-0C42-AA59-DF607BD5BD46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172A49B9-2968-324A-A0FE-5C98DC772FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16200" xr2:uid="{D513BC79-3938-9341-9AD1-4F90A265E8C7}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16200" activeTab="1" xr2:uid="{D513BC79-3938-9341-9AD1-4F90A265E8C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddVacancy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Uname</t>
   </si>
@@ -40,6 +41,66 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>job title</t>
+  </si>
+  <si>
+    <t>vacancy name</t>
+  </si>
+  <si>
+    <t>hiring manager</t>
+  </si>
+  <si>
+    <t>number of positions</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>test engineer</t>
+  </si>
+  <si>
+    <t>Kallyani Bhute</t>
+  </si>
+  <si>
+    <t>perform test using selenium in java</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>Paul Collings</t>
+  </si>
+  <si>
+    <t>part of team in assembly line</t>
+  </si>
+  <si>
+    <t>driver</t>
+  </si>
+  <si>
+    <t>Rebecca Harmony</t>
+  </si>
+  <si>
+    <t>AZ driver</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>Dominic Chase</t>
+  </si>
+  <si>
+    <t>frontend developer</t>
+  </si>
+  <si>
+    <t>analyst</t>
+  </si>
+  <si>
+    <t>Nathan Elliot</t>
+  </si>
+  <si>
+    <t>anylyse software feasibility</t>
   </si>
 </sst>
 </file>
@@ -75,8 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5320DD3-6646-5E41-9EA7-F54AE5374A97}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -434,4 +496,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D72129-856C-434D-B76D-A971B050A146}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>